<commit_message>
fixed locking of name
</commit_message>
<xml_diff>
--- a/144F20/Topic 2/Topic 2 Extra DQ 6.xlsx
+++ b/144F20/Topic 2/Topic 2 Extra DQ 6.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gcumail-my.sharepoint.com/personal/richard_ketchersid_gcu_edu/Documents/Course Materials/git/Teaching/144F20/Topic 2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:80_{BDBC4DFC-A303-4FF5-827A-07E85A60FF4D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:80_{7CBD9C24-F3B4-4033-B79A-2D9457AC7016}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1635" yWindow="1125" windowWidth="25995" windowHeight="14280" xr2:uid="{AF244846-4AAD-42AC-8F96-96B174BB4566}"/>
   </bookViews>
@@ -1363,6 +1363,154 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="47" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1410,12 +1558,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -1425,22 +1567,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -1492,137 +1618,13 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="47" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1630,16 +1632,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="3">
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <b/>
@@ -1653,6 +1645,16 @@
         <i val="0"/>
         <color rgb="FFFF0000"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2014,8 +2016,8 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{5C5BD3A8-4D62-4C95-94F7-358A1F622274}">
-  <header guid="{5C5BD3A8-4D62-4C95-94F7-358A1F622274}" dateTime="2021-09-30T13:21:14" maxSheetId="3" userName="Richard Ketchersid" r:id="rId1">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{F6743FB5-C608-414F-84BA-42B51547B24B}">
+  <header guid="{F6743FB5-C608-414F-84BA-42B51547B24B}" dateTime="2021-10-14T10:01:10" maxSheetId="3" userName="Richard Ketchersid" r:id="rId1">
     <sheetIdMap count="2">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -2030,7 +2032,7 @@
 
 <file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
 <users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="1">
-  <userInfo guid="{5C5BD3A8-4D62-4C95-94F7-358A1F622274}" name="Richard Ketchersid" id="-1739556524" dateTime="2021-09-30T13:21:14"/>
+  <userInfo guid="{F6743FB5-C608-414F-84BA-42B51547B24B}" name="Richard Ketchersid" id="-1739584685" dateTime="2021-10-14T10:01:10"/>
 </users>
 </file>
 
@@ -2334,7 +2336,7 @@
   <dimension ref="A1:N64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2345,107 +2347,107 @@
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="126" t="s">
+      <c r="A2" s="53" t="s">
         <v>80</v>
       </c>
-      <c r="B2" s="127"/>
-      <c r="C2" s="124" t="s">
+      <c r="B2" s="54"/>
+      <c r="C2" s="126" t="s">
         <v>81</v>
       </c>
-      <c r="D2" s="125"/>
+      <c r="D2" s="127"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="57" t="s">
+      <c r="A4" s="100" t="s">
         <v>77</v>
       </c>
-      <c r="B4" s="58"/>
-      <c r="C4" s="58"/>
-      <c r="D4" s="58"/>
-      <c r="E4" s="58"/>
-      <c r="F4" s="58"/>
-      <c r="G4" s="58"/>
-      <c r="H4" s="59"/>
+      <c r="B4" s="101"/>
+      <c r="C4" s="101"/>
+      <c r="D4" s="101"/>
+      <c r="E4" s="101"/>
+      <c r="F4" s="101"/>
+      <c r="G4" s="101"/>
+      <c r="H4" s="102"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="60"/>
-      <c r="B5" s="61"/>
-      <c r="C5" s="61"/>
-      <c r="D5" s="61"/>
-      <c r="E5" s="61"/>
-      <c r="F5" s="61"/>
-      <c r="G5" s="61"/>
-      <c r="H5" s="62"/>
+      <c r="A5" s="103"/>
+      <c r="B5" s="104"/>
+      <c r="C5" s="104"/>
+      <c r="D5" s="104"/>
+      <c r="E5" s="104"/>
+      <c r="F5" s="104"/>
+      <c r="G5" s="104"/>
+      <c r="H5" s="105"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="60"/>
-      <c r="B6" s="61"/>
-      <c r="C6" s="61"/>
-      <c r="D6" s="61"/>
-      <c r="E6" s="61"/>
-      <c r="F6" s="61"/>
-      <c r="G6" s="61"/>
-      <c r="H6" s="62"/>
+      <c r="A6" s="103"/>
+      <c r="B6" s="104"/>
+      <c r="C6" s="104"/>
+      <c r="D6" s="104"/>
+      <c r="E6" s="104"/>
+      <c r="F6" s="104"/>
+      <c r="G6" s="104"/>
+      <c r="H6" s="105"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="60"/>
-      <c r="B7" s="61"/>
-      <c r="C7" s="61"/>
-      <c r="D7" s="61"/>
-      <c r="E7" s="61"/>
-      <c r="F7" s="61"/>
-      <c r="G7" s="61"/>
-      <c r="H7" s="62"/>
+      <c r="A7" s="103"/>
+      <c r="B7" s="104"/>
+      <c r="C7" s="104"/>
+      <c r="D7" s="104"/>
+      <c r="E7" s="104"/>
+      <c r="F7" s="104"/>
+      <c r="G7" s="104"/>
+      <c r="H7" s="105"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="60"/>
-      <c r="B8" s="61"/>
-      <c r="C8" s="61"/>
-      <c r="D8" s="61"/>
-      <c r="E8" s="61"/>
-      <c r="F8" s="61"/>
-      <c r="G8" s="61"/>
-      <c r="H8" s="62"/>
+      <c r="A8" s="103"/>
+      <c r="B8" s="104"/>
+      <c r="C8" s="104"/>
+      <c r="D8" s="104"/>
+      <c r="E8" s="104"/>
+      <c r="F8" s="104"/>
+      <c r="G8" s="104"/>
+      <c r="H8" s="105"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="60"/>
-      <c r="B9" s="61"/>
-      <c r="C9" s="61"/>
-      <c r="D9" s="61"/>
-      <c r="E9" s="61"/>
-      <c r="F9" s="61"/>
-      <c r="G9" s="61"/>
-      <c r="H9" s="62"/>
+      <c r="A9" s="103"/>
+      <c r="B9" s="104"/>
+      <c r="C9" s="104"/>
+      <c r="D9" s="104"/>
+      <c r="E9" s="104"/>
+      <c r="F9" s="104"/>
+      <c r="G9" s="104"/>
+      <c r="H9" s="105"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="60"/>
-      <c r="B10" s="61"/>
-      <c r="C10" s="61"/>
-      <c r="D10" s="61"/>
-      <c r="E10" s="61"/>
-      <c r="F10" s="61"/>
-      <c r="G10" s="61"/>
-      <c r="H10" s="62"/>
+      <c r="A10" s="103"/>
+      <c r="B10" s="104"/>
+      <c r="C10" s="104"/>
+      <c r="D10" s="104"/>
+      <c r="E10" s="104"/>
+      <c r="F10" s="104"/>
+      <c r="G10" s="104"/>
+      <c r="H10" s="105"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="60"/>
-      <c r="B11" s="61"/>
-      <c r="C11" s="61"/>
-      <c r="D11" s="61"/>
-      <c r="E11" s="61"/>
-      <c r="F11" s="61"/>
-      <c r="G11" s="61"/>
-      <c r="H11" s="62"/>
+      <c r="A11" s="103"/>
+      <c r="B11" s="104"/>
+      <c r="C11" s="104"/>
+      <c r="D11" s="104"/>
+      <c r="E11" s="104"/>
+      <c r="F11" s="104"/>
+      <c r="G11" s="104"/>
+      <c r="H11" s="105"/>
     </row>
     <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="63"/>
-      <c r="B12" s="64"/>
-      <c r="C12" s="64"/>
-      <c r="D12" s="64"/>
-      <c r="E12" s="64"/>
-      <c r="F12" s="64"/>
-      <c r="G12" s="64"/>
-      <c r="H12" s="65"/>
+      <c r="A12" s="106"/>
+      <c r="B12" s="107"/>
+      <c r="C12" s="107"/>
+      <c r="D12" s="107"/>
+      <c r="E12" s="107"/>
+      <c r="F12" s="107"/>
+      <c r="G12" s="107"/>
+      <c r="H12" s="108"/>
     </row>
     <row r="14" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
@@ -2487,10 +2489,10 @@
         <v>6</v>
       </c>
       <c r="F15" s="2"/>
-      <c r="G15" s="71" t="s">
+      <c r="G15" s="112" t="s">
         <v>7</v>
       </c>
-      <c r="H15" s="72"/>
+      <c r="H15" s="113"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
@@ -2759,73 +2761,73 @@
       <c r="K26" s="2"/>
     </row>
     <row r="27" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="80" t="s">
+      <c r="A27" s="117" t="s">
         <v>58</v>
       </c>
-      <c r="B27" s="81"/>
-      <c r="C27" s="81"/>
-      <c r="D27" s="81"/>
-      <c r="E27" s="81"/>
-      <c r="F27" s="81"/>
-      <c r="G27" s="81"/>
-      <c r="H27" s="82"/>
+      <c r="B27" s="118"/>
+      <c r="C27" s="118"/>
+      <c r="D27" s="118"/>
+      <c r="E27" s="118"/>
+      <c r="F27" s="118"/>
+      <c r="G27" s="118"/>
+      <c r="H27" s="119"/>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" s="83"/>
-      <c r="B28" s="84"/>
-      <c r="C28" s="84"/>
-      <c r="D28" s="84"/>
-      <c r="E28" s="84"/>
-      <c r="F28" s="84"/>
-      <c r="G28" s="84"/>
-      <c r="H28" s="85"/>
+      <c r="A28" s="120"/>
+      <c r="B28" s="121"/>
+      <c r="C28" s="121"/>
+      <c r="D28" s="121"/>
+      <c r="E28" s="121"/>
+      <c r="F28" s="121"/>
+      <c r="G28" s="121"/>
+      <c r="H28" s="122"/>
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="83"/>
-      <c r="B29" s="84"/>
-      <c r="C29" s="84"/>
-      <c r="D29" s="84"/>
-      <c r="E29" s="84"/>
-      <c r="F29" s="84"/>
-      <c r="G29" s="84"/>
-      <c r="H29" s="85"/>
+      <c r="A29" s="120"/>
+      <c r="B29" s="121"/>
+      <c r="C29" s="121"/>
+      <c r="D29" s="121"/>
+      <c r="E29" s="121"/>
+      <c r="F29" s="121"/>
+      <c r="G29" s="121"/>
+      <c r="H29" s="122"/>
       <c r="I29" s="2"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="83"/>
-      <c r="B30" s="84"/>
-      <c r="C30" s="84"/>
-      <c r="D30" s="84"/>
-      <c r="E30" s="84"/>
-      <c r="F30" s="84"/>
-      <c r="G30" s="84"/>
-      <c r="H30" s="85"/>
+      <c r="A30" s="120"/>
+      <c r="B30" s="121"/>
+      <c r="C30" s="121"/>
+      <c r="D30" s="121"/>
+      <c r="E30" s="121"/>
+      <c r="F30" s="121"/>
+      <c r="G30" s="121"/>
+      <c r="H30" s="122"/>
       <c r="I30" s="2"/>
     </row>
     <row r="31" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="86"/>
-      <c r="B31" s="87"/>
-      <c r="C31" s="87"/>
-      <c r="D31" s="87"/>
-      <c r="E31" s="87"/>
-      <c r="F31" s="87"/>
-      <c r="G31" s="87"/>
-      <c r="H31" s="88"/>
+      <c r="A31" s="123"/>
+      <c r="B31" s="124"/>
+      <c r="C31" s="124"/>
+      <c r="D31" s="124"/>
+      <c r="E31" s="124"/>
+      <c r="F31" s="124"/>
+      <c r="G31" s="124"/>
+      <c r="H31" s="125"/>
       <c r="I31" s="2"/>
     </row>
     <row r="32" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="80" t="s">
+      <c r="A32" s="117" t="s">
         <v>60</v>
       </c>
-      <c r="B32" s="81"/>
-      <c r="C32" s="81"/>
-      <c r="D32" s="82"/>
+      <c r="B32" s="118"/>
+      <c r="C32" s="118"/>
+      <c r="D32" s="119"/>
       <c r="E32" s="32"/>
       <c r="F32" s="32"/>
       <c r="G32" s="32"/>
@@ -2836,60 +2838,60 @@
       <c r="L32" s="34"/>
     </row>
     <row r="33" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="83"/>
-      <c r="B33" s="84"/>
-      <c r="C33" s="84"/>
-      <c r="D33" s="85"/>
+      <c r="A33" s="120"/>
+      <c r="B33" s="121"/>
+      <c r="C33" s="121"/>
+      <c r="D33" s="122"/>
       <c r="E33" s="32"/>
-      <c r="F33" s="66" t="s">
+      <c r="F33" s="109" t="s">
         <v>71</v>
       </c>
-      <c r="G33" s="70"/>
-      <c r="H33" s="67"/>
+      <c r="G33" s="111"/>
+      <c r="H33" s="110"/>
       <c r="I33" s="2"/>
       <c r="J33" s="34"/>
       <c r="K33" s="34"/>
       <c r="L33" s="34"/>
     </row>
     <row r="34" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="105" t="s">
+      <c r="A34" s="70" t="s">
         <v>78</v>
       </c>
-      <c r="B34" s="106"/>
-      <c r="C34" s="106"/>
-      <c r="D34" s="107"/>
+      <c r="B34" s="71"/>
+      <c r="C34" s="71"/>
+      <c r="D34" s="72"/>
       <c r="E34" s="33"/>
-      <c r="F34" s="105" t="s">
+      <c r="F34" s="70" t="s">
         <v>79</v>
       </c>
-      <c r="G34" s="106"/>
-      <c r="H34" s="106"/>
-      <c r="I34" s="106"/>
-      <c r="J34" s="106"/>
-      <c r="K34" s="107"/>
+      <c r="G34" s="71"/>
+      <c r="H34" s="71"/>
+      <c r="I34" s="71"/>
+      <c r="J34" s="71"/>
+      <c r="K34" s="72"/>
     </row>
     <row r="35" spans="1:14" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="13"/>
-      <c r="B35" s="77" t="s">
+      <c r="B35" s="114" t="s">
         <v>32</v>
       </c>
-      <c r="C35" s="78"/>
-      <c r="D35" s="77" t="s">
+      <c r="C35" s="115"/>
+      <c r="D35" s="114" t="s">
         <v>44</v>
       </c>
-      <c r="E35" s="78"/>
-      <c r="F35" s="77" t="s">
+      <c r="E35" s="115"/>
+      <c r="F35" s="114" t="s">
         <v>46</v>
       </c>
-      <c r="G35" s="79"/>
-      <c r="H35" s="103" t="s">
+      <c r="G35" s="116"/>
+      <c r="H35" s="68" t="s">
         <v>54</v>
       </c>
-      <c r="I35" s="104"/>
-      <c r="J35" s="66" t="s">
+      <c r="I35" s="69"/>
+      <c r="J35" s="109" t="s">
         <v>72</v>
       </c>
-      <c r="K35" s="67"/>
+      <c r="K35" s="110"/>
       <c r="L35" s="48"/>
       <c r="M35" s="48"/>
     </row>
@@ -2927,36 +2929,36 @@
       <c r="K36" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="L36" s="54" t="s">
+      <c r="L36" s="97" t="s">
         <v>74</v>
       </c>
-      <c r="M36" s="55"/>
-      <c r="N36" s="56"/>
+      <c r="M36" s="98"/>
+      <c r="N36" s="99"/>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="B37" s="73" t="s">
+      <c r="B37" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="C37" s="74"/>
-      <c r="D37" s="75" t="s">
+      <c r="C37" s="58"/>
+      <c r="D37" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="E37" s="76"/>
-      <c r="F37" s="75" t="s">
+      <c r="E37" s="56"/>
+      <c r="F37" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="G37" s="76"/>
-      <c r="H37" s="75" t="s">
+      <c r="G37" s="56"/>
+      <c r="H37" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="I37" s="76"/>
-      <c r="J37" s="68" t="s">
+      <c r="I37" s="56"/>
+      <c r="J37" s="82" t="s">
         <v>35</v>
       </c>
-      <c r="K37" s="69"/>
+      <c r="K37" s="83"/>
     </row>
     <row r="38" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="14" t="s">
@@ -2981,26 +2983,26 @@
       <c r="A39" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="B39" s="73" t="s">
+      <c r="B39" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="C39" s="74"/>
-      <c r="D39" s="75" t="s">
+      <c r="C39" s="58"/>
+      <c r="D39" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="E39" s="76"/>
-      <c r="F39" s="75" t="s">
+      <c r="E39" s="56"/>
+      <c r="F39" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="G39" s="76"/>
-      <c r="H39" s="75" t="s">
+      <c r="G39" s="56"/>
+      <c r="H39" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="I39" s="76"/>
-      <c r="J39" s="68" t="s">
+      <c r="I39" s="56"/>
+      <c r="J39" s="82" t="s">
         <v>35</v>
       </c>
-      <c r="K39" s="69"/>
+      <c r="K39" s="83"/>
     </row>
     <row r="40" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="14" t="s">
@@ -3025,31 +3027,31 @@
       <c r="A41" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="B41" s="116"/>
-      <c r="C41" s="117"/>
-      <c r="D41" s="120"/>
-      <c r="E41" s="121"/>
-      <c r="F41" s="75" t="s">
+      <c r="B41" s="60"/>
+      <c r="C41" s="61"/>
+      <c r="D41" s="64"/>
+      <c r="E41" s="65"/>
+      <c r="F41" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="G41" s="76"/>
-      <c r="H41" s="75" t="s">
+      <c r="G41" s="56"/>
+      <c r="H41" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="I41" s="76"/>
-      <c r="J41" s="68" t="s">
+      <c r="I41" s="56"/>
+      <c r="J41" s="82" t="s">
         <v>35</v>
       </c>
-      <c r="K41" s="69"/>
+      <c r="K41" s="83"/>
     </row>
     <row r="42" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="B42" s="118"/>
-      <c r="C42" s="119"/>
-      <c r="D42" s="122"/>
-      <c r="E42" s="123"/>
+      <c r="B42" s="62"/>
+      <c r="C42" s="63"/>
+      <c r="D42" s="66"/>
+      <c r="E42" s="67"/>
       <c r="F42" s="17"/>
       <c r="G42" s="18"/>
       <c r="H42" s="17"/>
@@ -3061,26 +3063,26 @@
       <c r="A43" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B43" s="115" t="s">
+      <c r="B43" s="88" t="s">
         <v>2</v>
       </c>
-      <c r="C43" s="74"/>
-      <c r="D43" s="108" t="s">
+      <c r="C43" s="58"/>
+      <c r="D43" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="E43" s="76"/>
-      <c r="F43" s="108" t="s">
+      <c r="E43" s="56"/>
+      <c r="F43" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="G43" s="76"/>
-      <c r="H43" s="108" t="s">
+      <c r="G43" s="56"/>
+      <c r="H43" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="I43" s="76"/>
-      <c r="J43" s="68" t="s">
+      <c r="I43" s="56"/>
+      <c r="J43" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="K43" s="69"/>
+      <c r="K43" s="83"/>
     </row>
     <row r="44" spans="1:14" ht="53.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="20" t="s">
@@ -3103,16 +3105,16 @@
     </row>
     <row r="45" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="E46" s="109" t="s">
+      <c r="E46" s="76" t="s">
         <v>57</v>
       </c>
-      <c r="F46" s="110"/>
-      <c r="G46" s="111"/>
+      <c r="F46" s="77"/>
+      <c r="G46" s="78"/>
     </row>
     <row r="47" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E47" s="112"/>
-      <c r="F47" s="113"/>
-      <c r="G47" s="114"/>
+      <c r="E47" s="79"/>
+      <c r="F47" s="80"/>
+      <c r="G47" s="81"/>
     </row>
     <row r="48" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="49" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -3212,10 +3214,10 @@
       <c r="D53" s="42"/>
       <c r="E53" s="42"/>
       <c r="F53" s="42"/>
-      <c r="G53" s="97" t="s">
+      <c r="G53" s="84" t="s">
         <v>69</v>
       </c>
-      <c r="H53" s="99"/>
+      <c r="H53" s="85"/>
       <c r="I53" s="42"/>
       <c r="J53" s="42"/>
       <c r="K53" s="42"/>
@@ -3229,8 +3231,8 @@
       <c r="D54" s="42"/>
       <c r="E54" s="42"/>
       <c r="F54" s="42"/>
-      <c r="G54" s="100"/>
-      <c r="H54" s="102"/>
+      <c r="G54" s="86"/>
+      <c r="H54" s="87"/>
       <c r="I54" s="42"/>
       <c r="J54" s="42"/>
       <c r="K54" s="42"/>
@@ -3238,22 +3240,22 @@
       <c r="M54" s="43"/>
     </row>
     <row r="55" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="53">
+      <c r="A55" s="96">
         <v>34</v>
       </c>
       <c r="B55" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="C55" s="89" t="s">
+      <c r="C55" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="D55" s="95">
+      <c r="D55" s="75">
         <v>34</v>
       </c>
       <c r="E55" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="F55" s="96" t="s">
+      <c r="F55" s="74" t="s">
         <v>65</v>
       </c>
       <c r="G55" s="35">
@@ -3264,7 +3266,7 @@
         <f>F51</f>
         <v>bar</v>
       </c>
-      <c r="I55" s="96" t="s">
+      <c r="I55" s="74" t="s">
         <v>65</v>
       </c>
       <c r="J55" s="35">
@@ -3279,16 +3281,16 @@
       <c r="M55" s="43"/>
     </row>
     <row r="56" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="53"/>
+      <c r="A56" s="96"/>
       <c r="B56" s="44" t="s">
         <v>64</v>
       </c>
-      <c r="C56" s="96"/>
-      <c r="D56" s="95"/>
+      <c r="C56" s="74"/>
+      <c r="D56" s="75"/>
       <c r="E56" s="44" t="s">
         <v>64</v>
       </c>
-      <c r="F56" s="96"/>
+      <c r="F56" s="74"/>
       <c r="G56" s="44">
         <f>B51</f>
         <v>1.23</v>
@@ -3297,7 +3299,7 @@
         <f>C51</f>
         <v>baz</v>
       </c>
-      <c r="I56" s="96"/>
+      <c r="I56" s="74"/>
       <c r="J56" s="44">
         <f>B52</f>
         <v>5.67</v>
@@ -3327,64 +3329,64 @@
     <row r="58" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="41"/>
       <c r="B58" s="42"/>
-      <c r="C58" s="89" t="s">
+      <c r="C58" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="D58" s="96">
+      <c r="D58" s="74">
         <v>34</v>
       </c>
-      <c r="E58" s="96" t="s">
+      <c r="E58" s="74" t="s">
         <v>65</v>
       </c>
       <c r="F58" s="37">
         <f>E51</f>
         <v>2.2046199999999998</v>
       </c>
-      <c r="G58" s="96" t="s">
+      <c r="G58" s="74" t="s">
         <v>65</v>
       </c>
       <c r="H58" s="35">
         <f>E52</f>
         <v>29.573499999999999</v>
       </c>
-      <c r="I58" s="96" t="s">
+      <c r="I58" s="74" t="s">
         <v>65</v>
       </c>
-      <c r="J58" s="94" t="s">
+      <c r="J58" s="93" t="s">
         <v>66</v>
       </c>
-      <c r="K58" s="94"/>
+      <c r="K58" s="93"/>
       <c r="L58" s="42"/>
       <c r="M58" s="43"/>
     </row>
     <row r="59" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="90" t="s">
+      <c r="A59" s="89" t="s">
         <v>70</v>
       </c>
-      <c r="B59" s="91"/>
-      <c r="C59" s="89"/>
-      <c r="D59" s="96"/>
-      <c r="E59" s="96"/>
+      <c r="B59" s="90"/>
+      <c r="C59" s="73"/>
+      <c r="D59" s="74"/>
+      <c r="E59" s="74"/>
       <c r="F59" s="45">
         <f>B51</f>
         <v>1.23</v>
       </c>
-      <c r="G59" s="96"/>
+      <c r="G59" s="74"/>
       <c r="H59" s="44">
         <f>B52</f>
         <v>5.67</v>
       </c>
-      <c r="I59" s="96"/>
-      <c r="J59" s="95" t="s">
+      <c r="I59" s="74"/>
+      <c r="J59" s="75" t="s">
         <v>67</v>
       </c>
-      <c r="K59" s="95"/>
+      <c r="K59" s="75"/>
       <c r="L59" s="42"/>
       <c r="M59" s="43"/>
     </row>
     <row r="60" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="92"/>
-      <c r="B60" s="93"/>
+      <c r="A60" s="91"/>
+      <c r="B60" s="92"/>
       <c r="C60" s="42"/>
       <c r="D60" s="42"/>
       <c r="E60" s="42"/>
@@ -3400,10 +3402,10 @@
     <row r="61" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="41"/>
       <c r="B61" s="42"/>
-      <c r="C61" s="89" t="s">
+      <c r="C61" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="D61" s="96">
+      <c r="D61" s="74">
         <f>D58*E51/B51*E52/B52</f>
         <v>317.85365930801106</v>
       </c>
@@ -3414,18 +3416,18 @@
       <c r="G61" s="42"/>
       <c r="H61" s="42"/>
       <c r="I61" s="42"/>
-      <c r="J61" s="97" t="s">
+      <c r="J61" s="84" t="s">
         <v>68</v>
       </c>
-      <c r="K61" s="98"/>
-      <c r="L61" s="99"/>
+      <c r="K61" s="94"/>
+      <c r="L61" s="85"/>
       <c r="M61" s="43"/>
     </row>
     <row r="62" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="41"/>
       <c r="B62" s="42"/>
-      <c r="C62" s="89"/>
-      <c r="D62" s="96"/>
+      <c r="C62" s="73"/>
+      <c r="D62" s="74"/>
       <c r="E62" s="44" t="s">
         <v>63</v>
       </c>
@@ -3433,9 +3435,9 @@
       <c r="G62" s="42"/>
       <c r="H62" s="42"/>
       <c r="I62" s="42"/>
-      <c r="J62" s="100"/>
-      <c r="K62" s="101"/>
-      <c r="L62" s="102"/>
+      <c r="J62" s="86"/>
+      <c r="K62" s="95"/>
+      <c r="L62" s="87"/>
       <c r="M62" s="43"/>
     </row>
     <row r="63" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3455,25 +3457,42 @@
     </row>
     <row r="64" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="m6dV6Pagh1EIAZp6eIOlJpxXpN9k/ZsAfvxWGAXZp6E8Ef+FFVCGF1bxKnVyvY6xJG4gnqS5p06ZliQyKT2ouw==" saltValue="mL9lUQSxM6PtTTPoBE/axA==" spinCount="100000" sheet="1" formatCells="0" formatColumns="0" formatRows="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="yt0L1khnJIHTTxZ3qm9rDnHwditKfkR0F0CTyAboNG93Auvb9d/Nn5lJT/tZ/L1vh88WGQk37OxYVHvTFk3j/g==" saltValue="2hFy9qldaJDM3tGtYcbpMg==" spinCount="100000" sheet="1" formatCells="0" formatColumns="0" formatRows="0"/>
   <customSheetViews>
     <customSheetView guid="{D3B99D0F-5290-4C19-9294-325A292E8E9A}">
-      <selection activeCell="C38" sqref="C38"/>
+      <selection activeCell="C3" sqref="C3"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="53">
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="F39:G39"/>
-    <mergeCell ref="B41:C42"/>
-    <mergeCell ref="D41:E42"/>
-    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="A55:A56"/>
+    <mergeCell ref="L36:N36"/>
+    <mergeCell ref="A4:H12"/>
+    <mergeCell ref="J35:K35"/>
+    <mergeCell ref="J37:K37"/>
+    <mergeCell ref="F33:H33"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="H37:I37"/>
+    <mergeCell ref="A27:H31"/>
+    <mergeCell ref="A32:D33"/>
+    <mergeCell ref="C61:C62"/>
+    <mergeCell ref="A59:B60"/>
+    <mergeCell ref="J58:K58"/>
+    <mergeCell ref="J59:K59"/>
+    <mergeCell ref="D61:D62"/>
+    <mergeCell ref="J61:L62"/>
+    <mergeCell ref="C58:C59"/>
+    <mergeCell ref="D58:D59"/>
+    <mergeCell ref="E58:E59"/>
+    <mergeCell ref="G58:G59"/>
+    <mergeCell ref="I58:I59"/>
     <mergeCell ref="H35:I35"/>
     <mergeCell ref="F34:K34"/>
     <mergeCell ref="C55:C56"/>
@@ -3490,36 +3509,19 @@
     <mergeCell ref="G53:H54"/>
     <mergeCell ref="A34:D34"/>
     <mergeCell ref="B43:C43"/>
-    <mergeCell ref="C61:C62"/>
-    <mergeCell ref="A59:B60"/>
-    <mergeCell ref="J58:K58"/>
-    <mergeCell ref="J59:K59"/>
-    <mergeCell ref="D61:D62"/>
-    <mergeCell ref="J61:L62"/>
-    <mergeCell ref="C58:C59"/>
-    <mergeCell ref="D58:D59"/>
-    <mergeCell ref="E58:E59"/>
-    <mergeCell ref="G58:G59"/>
-    <mergeCell ref="I58:I59"/>
-    <mergeCell ref="A55:A56"/>
-    <mergeCell ref="L36:N36"/>
-    <mergeCell ref="A4:H12"/>
-    <mergeCell ref="J35:K35"/>
-    <mergeCell ref="J37:K37"/>
-    <mergeCell ref="F33:H33"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="F35:G35"/>
-    <mergeCell ref="H37:I37"/>
-    <mergeCell ref="A27:H31"/>
-    <mergeCell ref="A32:D33"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="B41:C42"/>
+    <mergeCell ref="D41:E42"/>
+    <mergeCell ref="F41:G41"/>
   </mergeCells>
   <conditionalFormatting sqref="A4:N68">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="2" priority="1">
       <formula>$C$2="Your Name Here"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3624,10 +3626,10 @@
         <v>6</v>
       </c>
       <c r="F12" s="2"/>
-      <c r="G12" s="71" t="s">
+      <c r="G12" s="112" t="s">
         <v>7</v>
       </c>
-      <c r="H12" s="72"/>
+      <c r="H12" s="113"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
@@ -3975,26 +3977,26 @@
     </row>
     <row r="30" spans="1:14" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="13"/>
-      <c r="B30" s="77" t="s">
+      <c r="B30" s="114" t="s">
         <v>32</v>
       </c>
-      <c r="C30" s="78"/>
-      <c r="D30" s="77" t="s">
+      <c r="C30" s="115"/>
+      <c r="D30" s="114" t="s">
         <v>44</v>
       </c>
-      <c r="E30" s="78"/>
-      <c r="F30" s="77" t="s">
+      <c r="E30" s="115"/>
+      <c r="F30" s="114" t="s">
         <v>46</v>
       </c>
-      <c r="G30" s="79"/>
-      <c r="H30" s="103" t="s">
+      <c r="G30" s="116"/>
+      <c r="H30" s="68" t="s">
         <v>54</v>
       </c>
-      <c r="I30" s="104"/>
-      <c r="J30" s="66" t="s">
+      <c r="I30" s="69"/>
+      <c r="J30" s="109" t="s">
         <v>72</v>
       </c>
-      <c r="K30" s="67"/>
+      <c r="K30" s="110"/>
       <c r="L30" s="48"/>
       <c r="M30" s="48"/>
     </row>
@@ -4032,36 +4034,36 @@
       <c r="K31" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="L31" s="54" t="s">
+      <c r="L31" s="97" t="s">
         <v>74</v>
       </c>
-      <c r="M31" s="55"/>
-      <c r="N31" s="56"/>
+      <c r="M31" s="98"/>
+      <c r="N31" s="99"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="B32" s="73" t="s">
+      <c r="B32" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="C32" s="74"/>
-      <c r="D32" s="75" t="s">
+      <c r="C32" s="58"/>
+      <c r="D32" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="E32" s="76"/>
-      <c r="F32" s="75" t="s">
+      <c r="E32" s="56"/>
+      <c r="F32" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="G32" s="76"/>
+      <c r="G32" s="56"/>
       <c r="H32" s="25" t="s">
         <v>35</v>
       </c>
       <c r="I32" s="29"/>
-      <c r="J32" s="68" t="s">
+      <c r="J32" s="82" t="s">
         <v>35</v>
       </c>
-      <c r="K32" s="69"/>
+      <c r="K32" s="83"/>
     </row>
     <row r="33" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
@@ -4106,26 +4108,26 @@
       <c r="A34" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="B34" s="73" t="s">
+      <c r="B34" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="C34" s="74"/>
-      <c r="D34" s="75" t="s">
+      <c r="C34" s="58"/>
+      <c r="D34" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="E34" s="76"/>
-      <c r="F34" s="75" t="s">
+      <c r="E34" s="56"/>
+      <c r="F34" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="G34" s="76"/>
+      <c r="G34" s="56"/>
       <c r="H34" s="25" t="s">
         <v>35</v>
       </c>
       <c r="I34" s="29"/>
-      <c r="J34" s="68" t="s">
+      <c r="J34" s="82" t="s">
         <v>35</v>
       </c>
-      <c r="K34" s="69"/>
+      <c r="K34" s="83"/>
     </row>
     <row r="35" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
@@ -4170,31 +4172,31 @@
       <c r="A36" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="B36" s="116"/>
-      <c r="C36" s="117"/>
-      <c r="D36" s="120"/>
-      <c r="E36" s="121"/>
-      <c r="F36" s="75" t="s">
+      <c r="B36" s="60"/>
+      <c r="C36" s="61"/>
+      <c r="D36" s="64"/>
+      <c r="E36" s="65"/>
+      <c r="F36" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="G36" s="76"/>
+      <c r="G36" s="56"/>
       <c r="H36" s="25" t="s">
         <v>35</v>
       </c>
       <c r="I36" s="29"/>
-      <c r="J36" s="68" t="s">
+      <c r="J36" s="82" t="s">
         <v>35</v>
       </c>
-      <c r="K36" s="69"/>
+      <c r="K36" s="83"/>
     </row>
     <row r="37" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="B37" s="118"/>
-      <c r="C37" s="119"/>
-      <c r="D37" s="122"/>
-      <c r="E37" s="123"/>
+      <c r="B37" s="62"/>
+      <c r="C37" s="63"/>
+      <c r="D37" s="66"/>
+      <c r="E37" s="67"/>
       <c r="F37" s="17">
         <f>D12/A12</f>
         <v>2.2046199999999998</v>
@@ -4221,26 +4223,26 @@
       <c r="A38" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B38" s="115" t="s">
+      <c r="B38" s="88" t="s">
         <v>2</v>
       </c>
-      <c r="C38" s="74"/>
-      <c r="D38" s="108" t="s">
+      <c r="C38" s="58"/>
+      <c r="D38" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="E38" s="76"/>
-      <c r="F38" s="108" t="s">
+      <c r="E38" s="56"/>
+      <c r="F38" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="G38" s="76"/>
+      <c r="G38" s="56"/>
       <c r="H38" s="26" t="s">
         <v>2</v>
       </c>
       <c r="I38" s="29"/>
-      <c r="J38" s="68" t="s">
+      <c r="J38" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="K38" s="69"/>
+      <c r="K38" s="83"/>
     </row>
     <row r="39" spans="1:11" ht="53.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="20" t="s">
@@ -4289,6 +4291,20 @@
     </customSheetView>
   </customSheetViews>
   <mergeCells count="23">
+    <mergeCell ref="J38:K38"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="L31:N31"/>
+    <mergeCell ref="J32:K32"/>
+    <mergeCell ref="J34:K34"/>
+    <mergeCell ref="J36:K36"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="H30:I30"/>
     <mergeCell ref="B38:C38"/>
     <mergeCell ref="D38:E38"/>
     <mergeCell ref="F38:G38"/>
@@ -4298,20 +4314,6 @@
     <mergeCell ref="B36:C37"/>
     <mergeCell ref="D36:E37"/>
     <mergeCell ref="F36:G36"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="J38:K38"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="L31:N31"/>
-    <mergeCell ref="J32:K32"/>
-    <mergeCell ref="J34:K34"/>
-    <mergeCell ref="J36:K36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>